<commit_message>
Update Sprint 2 report
</commit_message>
<xml_diff>
--- a/doc/Team2Report.xlsx
+++ b/doc/Team2Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kybeth/Documents/GitHub/SSW555-GEDCOM-Develop-Team02/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F264F38-5889-5B4D-8211-F887C471E106}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BDCACF-1434-A24F-8643-9C13B21A7EFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28380" windowHeight="15580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37720" yWindow="3400" windowWidth="28380" windowHeight="19920" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="224">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -729,6 +729,15 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Mess with the github</t>
+  </si>
+  <si>
+    <t>Start early</t>
+  </si>
+  <si>
+    <t>Refactor to use class structure and build automated test</t>
   </si>
 </sst>
 </file>
@@ -870,7 +879,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -908,6 +917,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="65">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1161,6 +1174,9 @@
                 <c:pt idx="1">
                   <c:v>42277</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>42291</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1175,6 +1191,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2064,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="B1:C6"/>
+    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2201,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3114,10 +3133,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3182,6 +3201,27 @@
         <v>19.047619047619047</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="2">
+        <v>42291</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>627</v>
+      </c>
+      <c r="E4">
+        <v>1090</v>
+      </c>
+      <c r="F4" s="9">
+        <f>(D4-D3)/E4*60</f>
+        <v>29.009174311926607</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3194,8 +3234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="C1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3626,14 +3666,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
@@ -3686,7 +3727,15 @@
       <c r="F2" s="20">
         <v>45</v>
       </c>
-      <c r="G2" s="20"/>
+      <c r="G2" s="20">
+        <v>23</v>
+      </c>
+      <c r="H2" s="20">
+        <v>360</v>
+      </c>
+      <c r="I2" s="22">
+        <v>42291</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
@@ -3707,7 +3756,15 @@
       <c r="F3" s="20">
         <v>45</v>
       </c>
-      <c r="G3" s="20"/>
+      <c r="G3" s="20">
+        <v>23</v>
+      </c>
+      <c r="H3" s="20">
+        <v>360</v>
+      </c>
+      <c r="I3" s="22">
+        <v>42291</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
@@ -3728,7 +3785,15 @@
       <c r="F4" s="20">
         <v>40</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="20">
+        <v>20</v>
+      </c>
+      <c r="H4" s="20">
+        <v>30</v>
+      </c>
+      <c r="I4" s="22">
+        <v>42291</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
@@ -3749,7 +3814,15 @@
       <c r="F5" s="20">
         <v>40</v>
       </c>
-      <c r="G5" s="20"/>
+      <c r="G5" s="20">
+        <v>15</v>
+      </c>
+      <c r="H5" s="20">
+        <v>30</v>
+      </c>
+      <c r="I5" s="22">
+        <v>42291</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -3770,7 +3843,15 @@
       <c r="F6" s="20">
         <v>40</v>
       </c>
-      <c r="G6" s="20"/>
+      <c r="G6" s="20">
+        <v>12</v>
+      </c>
+      <c r="H6" s="20">
+        <v>30</v>
+      </c>
+      <c r="I6" s="22">
+        <v>42291</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
@@ -3791,7 +3872,15 @@
       <c r="F7" s="20">
         <v>40</v>
       </c>
-      <c r="G7" s="20"/>
+      <c r="G7" s="20">
+        <v>11</v>
+      </c>
+      <c r="H7" s="20">
+        <v>30</v>
+      </c>
+      <c r="I7" s="22">
+        <v>42291</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
@@ -3812,7 +3901,15 @@
       <c r="F8" s="20">
         <v>30</v>
       </c>
-      <c r="G8" s="20"/>
+      <c r="G8" s="20">
+        <v>11</v>
+      </c>
+      <c r="H8" s="20">
+        <v>90</v>
+      </c>
+      <c r="I8" s="22">
+        <v>42291</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
@@ -3833,7 +3930,15 @@
       <c r="F9" s="20">
         <v>30</v>
       </c>
-      <c r="G9" s="20"/>
+      <c r="G9" s="20">
+        <v>13</v>
+      </c>
+      <c r="H9" s="20">
+        <v>60</v>
+      </c>
+      <c r="I9" s="22">
+        <v>42291</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
@@ -3854,7 +3959,15 @@
       <c r="F10" s="20">
         <v>30</v>
       </c>
-      <c r="G10" s="20"/>
+      <c r="G10" s="20">
+        <v>19</v>
+      </c>
+      <c r="H10" s="20">
+        <v>80</v>
+      </c>
+      <c r="I10" s="22">
+        <v>42291</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
@@ -3875,7 +3988,67 @@
       <c r="F11" s="20">
         <v>30</v>
       </c>
-      <c r="G11" s="20"/>
+      <c r="G11" s="20">
+        <v>20</v>
+      </c>
+      <c r="H11" s="20">
+        <v>20</v>
+      </c>
+      <c r="I11" s="22">
+        <v>42291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="H12">
+        <f xml:space="preserve"> SUM(H2:H11)</f>
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A14" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+      <c r="A15" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+      <c r="A16" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="43" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A20" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="42" x14ac:dyDescent="0.15">
+      <c r="A21" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="22" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="1" t="s">
+        <v>221</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3886,13 +4059,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
@@ -3921,6 +4099,206 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E10">
+        <v>18</v>
+      </c>
+      <c r="F10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E11">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3978,8 +4356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:B41"/>
+    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Update the class structure to add line_num to individual and family
</commit_message>
<xml_diff>
--- a/doc/Team2Report.xlsx
+++ b/doc/Team2Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kybeth/Documents/GitHub/SSW555-GEDCOM-Develop-Team02/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BDCACF-1434-A24F-8643-9C13B21A7EFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DDAEF4-CC7B-0545-9753-3AE298995E4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37720" yWindow="3400" windowWidth="28380" windowHeight="19920" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42080" yWindow="5660" windowWidth="28380" windowHeight="19920" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="242">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -738,6 +738,60 @@
   </si>
   <si>
     <t>Refactor to use class structure and build automated test</t>
+  </si>
+  <si>
+    <t>33-36</t>
+  </si>
+  <si>
+    <t>15-23</t>
+  </si>
+  <si>
+    <t>29-34</t>
+  </si>
+  <si>
+    <t>main.py</t>
+  </si>
+  <si>
+    <t>test.py</t>
+  </si>
+  <si>
+    <t>test_US22</t>
+  </si>
+  <si>
+    <t>test_US21</t>
+  </si>
+  <si>
+    <t>test_US23</t>
+  </si>
+  <si>
+    <t>test_US24</t>
+  </si>
+  <si>
+    <t>test_US25</t>
+  </si>
+  <si>
+    <t>test_US26</t>
+  </si>
+  <si>
+    <t>test_US27</t>
+  </si>
+  <si>
+    <t>test_US28</t>
+  </si>
+  <si>
+    <t>test_US29</t>
+  </si>
+  <si>
+    <t>test_US30</t>
+  </si>
+  <si>
+    <t>Write each one's code in different area to avoid conflicting</t>
+  </si>
+  <si>
+    <t>Spliting tasks in a sprint into smaller phases, and assign ddl to each phase</t>
+  </si>
+  <si>
+    <t>Writing tons of code without enough comments. This really makes it hard for team members to understand your code</t>
   </si>
 </sst>
 </file>
@@ -1177,6 +1231,9 @@
                 <c:pt idx="2">
                   <c:v>42291</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>42305</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1194,6 +1251,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2220,7 +2280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="150" workbookViewId="0">
       <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
@@ -3133,10 +3193,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3222,6 +3282,17 @@
         <v>29.009174311926607</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="2">
+        <v>42305</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3234,8 +3305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:R15"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4004,7 +4075,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>30</v>
       </c>
@@ -4017,7 +4088,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
         <v>31</v>
       </c>
@@ -4040,7 +4111,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="42" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:1" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>219</v>
       </c>
@@ -4059,10 +4130,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4072,7 +4143,7 @@
     <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4100,8 +4171,27 @@
       <c r="I1" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K1" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="L1" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="M1" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="N1" s="17"/>
+      <c r="O1" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -4120,8 +4210,33 @@
       <c r="F2">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G2">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="L2" t="s">
+        <v>132</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -4140,8 +4255,29 @@
       <c r="F3">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G3">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>120</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="L3" t="s">
+        <v>133</v>
+      </c>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q3" s="17"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>134</v>
       </c>
@@ -4160,8 +4296,32 @@
       <c r="F4">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+      <c r="I4" s="22">
+        <v>42304</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="L4" t="s">
+        <v>134</v>
+      </c>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="P4" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q4" s="17"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>135</v>
       </c>
@@ -4180,8 +4340,32 @@
       <c r="F5">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G5">
+        <v>17</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
+      <c r="I5" s="22">
+        <v>42304</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="L5" t="s">
+        <v>135</v>
+      </c>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q5" s="17"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -4200,13 +4384,34 @@
       <c r="F6">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="L6" t="s">
+        <v>136</v>
+      </c>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q6" s="17"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
         <v>185</v>
@@ -4220,8 +4425,29 @@
       <c r="F7">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="L7" t="s">
+        <v>137</v>
+      </c>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q7" s="17"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>138</v>
       </c>
@@ -4240,8 +4466,36 @@
       <c r="F8">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G8">
+        <v>11</v>
+      </c>
+      <c r="H8">
+        <v>15</v>
+      </c>
+      <c r="I8" s="22">
+        <v>42304</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="L8" t="s">
+        <v>138</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="N8" s="17"/>
+      <c r="O8" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q8" s="18" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>139</v>
       </c>
@@ -4260,8 +4514,32 @@
       <c r="F9">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G9">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9" s="22">
+        <v>42304</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="L9" t="s">
+        <v>139</v>
+      </c>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="P9" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q9" s="17"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>140</v>
       </c>
@@ -4280,8 +4558,32 @@
       <c r="F10">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
+      <c r="I10" s="22">
+        <v>42304</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="L10" t="s">
+        <v>140</v>
+      </c>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q10" s="17"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -4300,6 +4602,78 @@
       <c r="F11">
         <v>60</v>
       </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>15</v>
+      </c>
+      <c r="I11" s="22">
+        <v>42304</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="L11" t="s">
+        <v>141</v>
+      </c>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="P11" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q11" s="17"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+    </row>
+    <row r="14" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+      <c r="B14" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.15">
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="42" x14ac:dyDescent="0.15">
+      <c r="B17" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="42" x14ac:dyDescent="0.15">
+      <c r="B18" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
+      <c r="B20" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="70" x14ac:dyDescent="0.15">
+      <c r="B21" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B22" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4309,13 +4683,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
@@ -4344,6 +4722,170 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -4356,8 +4898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
modify us, separate test file
modify us09 10 19 20 29 30
separate Yuan's test  code into test_yz.py
made new test gedcom
</commit_message>
<xml_diff>
--- a/doc/Team2Report.xlsx
+++ b/doc/Team2Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kybeth/Documents/GitHub/SSW555-GEDCOM-Develop-Team02/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DDAEF4-CC7B-0545-9753-3AE298995E4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635F7F91-0118-DC4D-AC33-8640EFAB2FB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42080" yWindow="5660" windowWidth="28380" windowHeight="19920" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40420" yWindow="5660" windowWidth="28380" windowHeight="19920" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -4132,7 +4132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -4695,7 +4695,7 @@
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4898,8 +4898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>